<commit_message>
Restructuring. master refactor. final
</commit_message>
<xml_diff>
--- a/dir/users.xlsx
+++ b/dir/users.xlsx
@@ -15,69 +15,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
-  <si>
-    <t xml:space="preserve">Usuarios Cadastrados </t>
-  </si>
-  <si>
-    <t>Nome Completo</t>
-  </si>
-  <si>
-    <t>Data Nascimento</t>
-  </si>
-  <si>
-    <t>Email usuario</t>
-  </si>
-  <si>
-    <t>Link Facebook</t>
-  </si>
-  <si>
-    <t>RG Usuario</t>
-  </si>
-  <si>
-    <t>CPF Usuario</t>
-  </si>
-  <si>
-    <t>Endereco Usuario</t>
-  </si>
-  <si>
-    <t>CEP Usuario</t>
-  </si>
-  <si>
-    <t>Fone Usuario</t>
-  </si>
-  <si>
-    <t>Teste Sbobrenome Teste</t>
-  </si>
-  <si>
-    <t>1997-01-01</t>
-  </si>
-  <si>
-    <t>teste@teste.com.br</t>
-  </si>
-  <si>
-    <t>facebook.com/teste</t>
-  </si>
-  <si>
-    <t>11.111.111-1</t>
-  </si>
-  <si>
-    <t>367.388.308-90</t>
-  </si>
-  <si>
-    <t>Rua Teste Testeiros, numero 90</t>
-  </si>
-  <si>
-    <t>55555-555</t>
-  </si>
-  <si>
-    <t>(11) 44444-4444</t>
-  </si>
-  <si>
-    <t>22222-222</t>
-  </si>
-  <si>
-    <t>(22) 22222-2222</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>postal</t>
+  </si>
+  <si>
+    <t>fone</t>
+  </si>
+  <si>
+    <t>Brian Livramento</t>
+  </si>
+  <si>
+    <t>brian.livramento@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -85,7 +46,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="1">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -95,35 +56,8 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,18 +70,6 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -155,21 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="4" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,142 +380,60 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.83203125" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="true" style="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="true" style="1"/>
-    <col min="3" max="3" width="34.1640625" customWidth="true" style="1"/>
-    <col min="4" max="4" width="34.6640625" customWidth="true" style="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="true" style="1"/>
-    <col min="6" max="6" width="23.5" customWidth="true" style="1"/>
-    <col min="7" max="7" width="34.33203125" customWidth="true" style="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="true" style="1"/>
-    <col min="9" max="9" width="29.33203125" customWidth="true" style="1"/>
-    <col min="10" max="10" width="8.83203125" style="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:10" customHeight="1" ht="34">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" customHeight="1" ht="10">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
     </row>
-    <row r="3" spans="1:10" customHeight="1" ht="21">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="B3"/>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
-    <mergeCell ref="A1:I1"/>
-  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>

</xml_diff>